<commit_message>
updated animal stats to reflect simulated values
</commit_message>
<xml_diff>
--- a/data/animal_characteristics.xlsx
+++ b/data/animal_characteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\Stuff\Programing\Python\University Python\sim&amp;mod\Simulation-of-Ecosystem-Food-Chains\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3DC7B8-B391-4C3B-B550-661584095F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81B2B0D-9A4A-401C-9D42-ECDDEAEA955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9217EBFD-B9E8-4E74-AE9F-5EAED0C062D6}"/>
+    <workbookView xWindow="-28920" yWindow="615" windowWidth="29040" windowHeight="15720" xr2:uid="{9217EBFD-B9E8-4E74-AE9F-5EAED0C062D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Animals</t>
   </si>
@@ -74,22 +74,52 @@
     <t>Mouse</t>
   </si>
   <si>
-    <t>Max Hunger</t>
-  </si>
-  <si>
-    <t>Max Thirst</t>
-  </si>
-  <si>
-    <t>Max Exhaustion</t>
-  </si>
-  <si>
-    <t>Sleep Length</t>
-  </si>
-  <si>
-    <t>Min Hunger</t>
-  </si>
-  <si>
-    <t>Min Thirst</t>
+    <t>Min Hunger (ticks)</t>
+  </si>
+  <si>
+    <t>Max Hunger (ticks)</t>
+  </si>
+  <si>
+    <t>Min Thirst (ticks)</t>
+  </si>
+  <si>
+    <t>Max Thirst (ticks)</t>
+  </si>
+  <si>
+    <t>Max Exhaustion (ticks)</t>
+  </si>
+  <si>
+    <t>Sleep Length (ticks)</t>
+  </si>
+  <si>
+    <t>In game time (ticks)</t>
+  </si>
+  <si>
+    <t>In game time (seconds)</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>Detection Multiplier (constant)</t>
+  </si>
+  <si>
+    <t>Sight Range (pixels)</t>
+  </si>
+  <si>
+    <t>Procreation Cooldown (ticks)</t>
   </si>
 </sst>
 </file>
@@ -125,9 +155,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -444,149 +477,532 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2475D5EA-4E7E-4717-902A-695A9A7421B4}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="14" style="1" customWidth="1"/>
-    <col min="5" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="C2" s="1">
+        <f>D2/6</f>
+        <v>10080</v>
+      </c>
+      <c r="D2" s="1">
+        <f>O2*7</f>
+        <v>60480</v>
+      </c>
+      <c r="E2" s="1">
+        <f>F2/6</f>
+        <v>4320</v>
+      </c>
+      <c r="F2" s="1">
+        <f>O2*3</f>
+        <v>25920</v>
+      </c>
+      <c r="G2" s="1">
+        <f>O2*2</f>
+        <v>17280</v>
+      </c>
+      <c r="H2" s="1">
+        <f>O3*8</f>
+        <v>2880</v>
+      </c>
+      <c r="I2" s="1">
+        <f>I10*3</f>
+        <v>181440</v>
+      </c>
+      <c r="J2" s="1">
+        <f>J6*0.75</f>
+        <v>300</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
         <v>68</v>
       </c>
-      <c r="C2" s="1">
-        <v>3.8</v>
+      <c r="N2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="2">
+        <v>8640</v>
+      </c>
+      <c r="P2" s="1">
+        <f>O2/30</f>
+        <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C10" si="0">D3/6</f>
+        <v>7200</v>
+      </c>
+      <c r="D3" s="1">
+        <f>O2*5</f>
+        <v>43200</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E10" si="1">F3/6</f>
+        <v>2880</v>
+      </c>
+      <c r="F3" s="1">
+        <f>O2*2</f>
+        <v>17280</v>
+      </c>
+      <c r="G3" s="1">
+        <f>O3*12</f>
+        <v>4320</v>
+      </c>
+      <c r="H3" s="1">
+        <f>O3*2</f>
+        <v>720</v>
+      </c>
+      <c r="I3" s="1">
+        <f>I10*3</f>
+        <v>181440</v>
+      </c>
+      <c r="J3" s="1">
+        <f>J6*0.9</f>
+        <v>360</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
         <v>64</v>
       </c>
-      <c r="C3" s="1">
-        <v>1.8</v>
+      <c r="N3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="1">
+        <f>O2/24</f>
+        <v>360</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P5" si="2">O3/30</f>
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>14400</v>
+      </c>
+      <c r="D4" s="1">
+        <f>O2*10</f>
+        <v>86400</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>720</v>
+      </c>
+      <c r="F4" s="1">
+        <f>O3*12</f>
+        <v>4320</v>
+      </c>
+      <c r="G4" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="H4" s="1">
+        <f>O3</f>
+        <v>360</v>
+      </c>
+      <c r="I4" s="1">
+        <f>I10*1.2</f>
+        <v>72576</v>
+      </c>
+      <c r="J4" s="1">
+        <f>J6*0.25</f>
+        <v>100</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
         <v>16</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.02</v>
+      <c r="N4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="1">
+        <f>O3/60</f>
+        <v>6</v>
+      </c>
+      <c r="P4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>20160</v>
+      </c>
+      <c r="D5" s="1">
+        <f>O2*14</f>
+        <v>120960</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+      <c r="F5" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="G5" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="H5" s="1">
+        <f>O3*4</f>
+        <v>1440</v>
+      </c>
+      <c r="I5" s="1">
+        <f>I10*1.5</f>
+        <v>90720</v>
+      </c>
+      <c r="J5" s="1">
+        <f>J6*0.3</f>
+        <v>120</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
         <v>29</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.25</v>
+      <c r="N5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="1">
+        <f>O4/60</f>
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3333333333333335E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>5760</v>
+      </c>
+      <c r="D6" s="1">
+        <f>O2*4</f>
+        <v>34560</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+      <c r="F6" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="G6" s="1">
+        <f>O3*30</f>
+        <v>10800</v>
+      </c>
+      <c r="H6" s="1">
+        <f>O3*8</f>
+        <v>2880</v>
+      </c>
+      <c r="I6" s="1">
+        <f>I10*3</f>
+        <v>181440</v>
+      </c>
+      <c r="J6" s="1">
+        <v>400</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
         <v>100</v>
       </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+      <c r="D7" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+      <c r="F7" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="G7" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="H7" s="1">
+        <f>O3*8</f>
+        <v>2880</v>
+      </c>
+      <c r="I7" s="1">
+        <f>I10*2</f>
+        <v>120960</v>
+      </c>
+      <c r="J7" s="1">
+        <f>J6*0.6</f>
+        <v>240</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
         <v>40</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.03</v>
-      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+      <c r="D8" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+      <c r="F8" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="G8" s="1">
+        <f>O3*12</f>
+        <v>4320</v>
+      </c>
+      <c r="H8" s="1">
+        <f>O3*2</f>
+        <v>720</v>
+      </c>
+      <c r="I8" s="1">
+        <f>I10*1.1</f>
+        <v>66528</v>
+      </c>
+      <c r="J8" s="1">
+        <f>J6*0.5</f>
+        <v>200</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
         <v>40</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>4320</v>
+      </c>
+      <c r="D9" s="1">
+        <f>O2*3</f>
+        <v>25920</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+      <c r="F9" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="G9" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="H9" s="1">
+        <f>O3*6</f>
+        <v>2160</v>
+      </c>
+      <c r="I9" s="1">
+        <f>I10*0.75</f>
+        <v>45360</v>
+      </c>
+      <c r="J9" s="1">
+        <f>J6*0.15</f>
+        <v>60</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
         <v>15</v>
       </c>
-      <c r="C9" s="1">
-        <v>1E-4</v>
-      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>1440</v>
+      </c>
+      <c r="D10" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+      <c r="F10" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="G10" s="1">
+        <f>O2</f>
+        <v>8640</v>
+      </c>
+      <c r="H10" s="1">
+        <f>O3*6</f>
+        <v>2160</v>
+      </c>
+      <c r="I10" s="1">
+        <f>O2*7</f>
+        <v>60480</v>
+      </c>
+      <c r="J10" s="1">
+        <f>J6*0.45</f>
+        <v>180</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
         <v>12.87</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed speeds to match ingame requirements
</commit_message>
<xml_diff>
--- a/data/animal_characteristics.xlsx
+++ b/data/animal_characteristics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\Stuff\Programing\Python\University Python\sim&amp;mod\Simulation-of-Ecosystem-Food-Chains\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81B2B0D-9A4A-401C-9D42-ECDDEAEA955D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978928A4-A0CB-4F2C-BB17-E562E0465C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="615" windowWidth="29040" windowHeight="15720" xr2:uid="{9217EBFD-B9E8-4E74-AE9F-5EAED0C062D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Animals</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Fox</t>
   </si>
   <si>
-    <t>Top Speed (km/h)</t>
-  </si>
-  <si>
     <t>Avg Mass (kg)</t>
   </si>
   <si>
@@ -120,6 +117,12 @@
   </si>
   <si>
     <t>Procreation Cooldown (ticks)</t>
+  </si>
+  <si>
+    <t>Top Speed (px/t)</t>
+  </si>
+  <si>
+    <t>Min Speed (px/t)</t>
   </si>
 </sst>
 </file>
@@ -155,19 +158,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -477,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2475D5EA-4E7E-4717-902A-695A9A7421B4}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:K10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,59 +509,64 @@
     <col min="10" max="10" width="22.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="28.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="17.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -561,7 +578,7 @@
         <v>10080</v>
       </c>
       <c r="D2" s="1">
-        <f>O2*7</f>
+        <f>P2*7</f>
         <v>60480</v>
       </c>
       <c r="E2" s="1">
@@ -569,15 +586,15 @@
         <v>4320</v>
       </c>
       <c r="F2" s="1">
-        <f>O2*3</f>
+        <f>P2*3</f>
         <v>25920</v>
       </c>
       <c r="G2" s="1">
-        <f>O2*2</f>
+        <f>P2*2</f>
         <v>17280</v>
       </c>
       <c r="H2" s="1">
-        <f>O3*8</f>
+        <f>P3*8</f>
         <v>2880</v>
       </c>
       <c r="I2" s="1">
@@ -592,22 +609,27 @@
         <v>1</v>
       </c>
       <c r="L2" s="1">
-        <v>68</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="2">
-        <v>8640</v>
+        <f>L6*0.68</f>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="M2">
+        <f>L2/2</f>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="P2" s="1">
-        <f>O2/30</f>
+        <v>8640</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>P2/30</f>
         <v>288</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>1.8</v>
@@ -617,7 +639,7 @@
         <v>7200</v>
       </c>
       <c r="D3" s="1">
-        <f>O2*5</f>
+        <f>P2*5</f>
         <v>43200</v>
       </c>
       <c r="E3" s="1">
@@ -625,15 +647,15 @@
         <v>2880</v>
       </c>
       <c r="F3" s="1">
-        <f>O2*2</f>
+        <f>P2*2</f>
         <v>17280</v>
       </c>
       <c r="G3" s="1">
-        <f>O3*12</f>
+        <f>P3*12</f>
         <v>4320</v>
       </c>
       <c r="H3" s="1">
-        <f>O3*2</f>
+        <f>P3*2</f>
         <v>720</v>
       </c>
       <c r="I3" s="1">
@@ -648,23 +670,28 @@
         <v>1</v>
       </c>
       <c r="L3" s="1">
-        <v>64</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="1">
-        <f>O2/24</f>
+        <f>L6*0.64</f>
+        <v>6.4</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M10" si="2">L3/2</f>
+        <v>3.2</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="1">
+        <f>P2/24</f>
         <v>360</v>
       </c>
-      <c r="P3" s="1">
-        <f t="shared" ref="P3:P5" si="2">O3/30</f>
+      <c r="Q3" s="1">
+        <f t="shared" ref="Q3:Q5" si="3">P3/30</f>
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>0.02</v>
@@ -674,7 +701,7 @@
         <v>14400</v>
       </c>
       <c r="D4" s="1">
-        <f>O2*10</f>
+        <f>P2*10</f>
         <v>86400</v>
       </c>
       <c r="E4" s="1">
@@ -682,15 +709,15 @@
         <v>720</v>
       </c>
       <c r="F4" s="1">
-        <f>O3*12</f>
+        <f>P3*12</f>
         <v>4320</v>
       </c>
       <c r="G4" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="H4" s="1">
-        <f>O3</f>
+        <f>P3</f>
         <v>360</v>
       </c>
       <c r="I4" s="1">
@@ -705,23 +732,28 @@
         <v>1</v>
       </c>
       <c r="L4" s="1">
-        <v>16</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="1">
-        <f>O3/60</f>
+        <f>L6*0.16</f>
+        <v>1.6</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="1">
+        <f>P3/60</f>
         <v>6</v>
       </c>
-      <c r="P4" s="1">
-        <f t="shared" si="2"/>
+      <c r="Q4" s="1">
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>0.25</v>
@@ -731,7 +763,7 @@
         <v>20160</v>
       </c>
       <c r="D5" s="1">
-        <f>O2*14</f>
+        <f>P2*14</f>
         <v>120960</v>
       </c>
       <c r="E5" s="1">
@@ -739,15 +771,15 @@
         <v>1440</v>
       </c>
       <c r="F5" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="G5" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="H5" s="1">
-        <f>O3*4</f>
+        <f>P3*4</f>
         <v>1440</v>
       </c>
       <c r="I5" s="1">
@@ -762,23 +794,28 @@
         <v>1</v>
       </c>
       <c r="L5" s="1">
-        <v>29</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" s="1">
-        <f>O4/60</f>
+        <f>L6*0.29</f>
+        <v>2.9</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>1.45</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="1">
+        <f>P4/60</f>
         <v>0.1</v>
       </c>
-      <c r="P5" s="1">
-        <f t="shared" si="2"/>
+      <c r="Q5" s="1">
+        <f t="shared" si="3"/>
         <v>3.3333333333333335E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -788,7 +825,7 @@
         <v>5760</v>
       </c>
       <c r="D6" s="1">
-        <f>O2*4</f>
+        <f>P2*4</f>
         <v>34560</v>
       </c>
       <c r="E6" s="1">
@@ -796,15 +833,15 @@
         <v>1440</v>
       </c>
       <c r="F6" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="G6" s="1">
-        <f>O3*30</f>
+        <f>P3*30</f>
         <v>10800</v>
       </c>
       <c r="H6" s="1">
-        <f>O3*8</f>
+        <f>P3*8</f>
         <v>2880</v>
       </c>
       <c r="I6" s="1">
@@ -818,12 +855,16 @@
         <v>1</v>
       </c>
       <c r="L6" s="1">
-        <v>100</v>
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>0.03</v>
@@ -833,7 +874,7 @@
         <v>1440</v>
       </c>
       <c r="D7" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="E7" s="1">
@@ -841,15 +882,15 @@
         <v>1440</v>
       </c>
       <c r="F7" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="G7" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="H7" s="1">
-        <f>O3*8</f>
+        <f>P3*8</f>
         <v>2880</v>
       </c>
       <c r="I7" s="1">
@@ -864,12 +905,17 @@
         <v>1</v>
       </c>
       <c r="L7" s="1">
-        <v>40</v>
+        <f>L6*0.4</f>
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -879,7 +925,7 @@
         <v>1440</v>
       </c>
       <c r="D8" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="E8" s="1">
@@ -887,15 +933,15 @@
         <v>1440</v>
       </c>
       <c r="F8" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="G8" s="1">
-        <f>O3*12</f>
+        <f>P3*12</f>
         <v>4320</v>
       </c>
       <c r="H8" s="1">
-        <f>O3*2</f>
+        <f>P3*2</f>
         <v>720</v>
       </c>
       <c r="I8" s="1">
@@ -910,12 +956,17 @@
         <v>1</v>
       </c>
       <c r="L8" s="1">
-        <v>40</v>
+        <f>L6*0.4</f>
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>1E-4</v>
@@ -925,7 +976,7 @@
         <v>4320</v>
       </c>
       <c r="D9" s="1">
-        <f>O2*3</f>
+        <f>P2*3</f>
         <v>25920</v>
       </c>
       <c r="E9" s="1">
@@ -933,15 +984,15 @@
         <v>1440</v>
       </c>
       <c r="F9" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="G9" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="H9" s="1">
-        <f>O3*6</f>
+        <f>P3*6</f>
         <v>2160</v>
       </c>
       <c r="I9" s="1">
@@ -956,12 +1007,17 @@
         <v>1</v>
       </c>
       <c r="L9" s="1">
-        <v>15</v>
+        <f>L6*0.15</f>
+        <v>1.5</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>0.03</v>
@@ -971,7 +1027,7 @@
         <v>1440</v>
       </c>
       <c r="D10" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="E10" s="1">
@@ -979,19 +1035,19 @@
         <v>1440</v>
       </c>
       <c r="F10" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="G10" s="1">
-        <f>O2</f>
+        <f>P2</f>
         <v>8640</v>
       </c>
       <c r="H10" s="1">
-        <f>O3*6</f>
+        <f>P3*6</f>
         <v>2160</v>
       </c>
       <c r="I10" s="1">
-        <f>O2*7</f>
+        <f>P2*7</f>
         <v>60480</v>
       </c>
       <c r="J10" s="1">
@@ -1002,10 +1058,20 @@
         <v>1</v>
       </c>
       <c r="L10" s="1">
-        <v>12.87</v>
+        <f>L6*0.128</f>
+        <v>1.28</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>0.64</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>"MOD(ROW(),2)=1"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>